<commit_message>
new pictures hindex and citations evaluation
</commit_message>
<xml_diff>
--- a/images/citations.xlsx
+++ b/images/citations.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacques.klein/GoogleDrive/teamRepositories/myWebPage/jacquesklein2302.github.io/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacques.klein/jacquesklein2302.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E4D030-28E4-174C-8D5B-54F7D4004349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B37FF04-2011-454C-95E5-25ECB59397D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13940" yWindow="1840" windowWidth="33660" windowHeight="20360" xr2:uid="{ACB19145-8E22-7D4E-9954-B957022569C7}"/>
+    <workbookView xWindow="2340" yWindow="1620" windowWidth="33660" windowHeight="20360" xr2:uid="{ACB19145-8E22-7D4E-9954-B957022569C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -55,6 +55,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,11 +89,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -189,10 +203,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$126</c:f>
+              <c:f>Sheet1!$A$5:$A$149</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="122"/>
+                <c:ptCount val="145"/>
                 <c:pt idx="0">
                   <c:v>40848</c:v>
                 </c:pt>
@@ -558,16 +572,85 @@
                 </c:pt>
                 <c:pt idx="121">
                   <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>44835</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>44866</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>44896</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>44927</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>44958</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>44986</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>45017</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>45047</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>45078</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>45108</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>45139</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>45170</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>45200</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>45231</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$126</c:f>
+              <c:f>Sheet1!$B$5:$B$149</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="122"/>
+                <c:ptCount val="145"/>
                 <c:pt idx="0">
                   <c:v>329</c:v>
                 </c:pt>
@@ -600,6 +683,12 @@
                 </c:pt>
                 <c:pt idx="121">
                   <c:v>10121</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>11613</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>13717</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -872,10 +961,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$126</c:f>
+              <c:f>Sheet1!$A$5:$A$149</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="122"/>
+                <c:ptCount val="145"/>
                 <c:pt idx="0">
                   <c:v>40848</c:v>
                 </c:pt>
@@ -1241,16 +1330,85 @@
                 </c:pt>
                 <c:pt idx="121">
                   <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>44835</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>44866</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>44896</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>44927</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>44958</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>44986</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>45017</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>45047</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>45078</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>45108</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>45139</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>45170</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>45200</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>45231</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$126</c:f>
+              <c:f>Sheet1!$C$5:$C$149</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="122"/>
+                <c:ptCount val="145"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
@@ -1283,6 +1441,12 @@
                 </c:pt>
                 <c:pt idx="121">
                   <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4092,10 +4256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CD39B4-C474-484D-A525-0FA885BAEB22}">
-  <dimension ref="A4:D130"/>
+  <dimension ref="A4:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B126" sqref="B126:B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4810,10 +4974,10 @@
       <c r="A126" s="1">
         <v>44531</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="4">
         <v>10121</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="4">
         <v>48</v>
       </c>
       <c r="D126">
@@ -4824,20 +4988,212 @@
       <c r="A127" s="1">
         <v>44562</v>
       </c>
+      <c r="B127" s="5"/>
+      <c r="C127" s="5"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>44593</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B128" s="5"/>
+      <c r="C128" s="5"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>44621</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>44652</v>
+      </c>
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B131" s="5"/>
+      <c r="C131" s="5"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B133" s="5"/>
+      <c r="C133" s="5"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>44774</v>
+      </c>
+      <c r="B134" s="5"/>
+      <c r="C134" s="5"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>44805</v>
+      </c>
+      <c r="B135" s="4">
+        <v>11613</v>
+      </c>
+      <c r="C135" s="4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>44835</v>
+      </c>
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>44866</v>
+      </c>
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>44896</v>
+      </c>
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>44927</v>
+      </c>
+      <c r="B139" s="5"/>
+      <c r="C139" s="5"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>44958</v>
+      </c>
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>44986</v>
+      </c>
+      <c r="B141" s="5"/>
+      <c r="C141" s="5"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>45017</v>
+      </c>
+      <c r="B142" s="5"/>
+      <c r="C142" s="5"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>45078</v>
+      </c>
+      <c r="B144" s="5"/>
+      <c r="C144" s="5"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>45108</v>
+      </c>
+      <c r="B145" s="5"/>
+      <c r="C145" s="5"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>45139</v>
+      </c>
+      <c r="B146" s="5"/>
+      <c r="C146" s="5"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>45170</v>
+      </c>
+      <c r="B147" s="5"/>
+      <c r="C147" s="5"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B148" s="4">
+        <v>13717</v>
+      </c>
+      <c r="C148" s="4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>45231</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>45383</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>45444</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>45474</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>45505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update images for statistics
</commit_message>
<xml_diff>
--- a/images/citations.xlsx
+++ b/images/citations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacques.klein/jacquesklein2302.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B37FF04-2011-454C-95E5-25ECB59397D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBD65C9-F639-D74F-B3E6-3EBAAB5D77B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="1620" windowWidth="33660" windowHeight="20360" xr2:uid="{ACB19145-8E22-7D4E-9954-B957022569C7}"/>
   </bookViews>
@@ -116,7 +116,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -203,10 +203,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$149</c:f>
+              <c:f>Sheet1!$A$5:$A$174</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="145"/>
+                <c:ptCount val="170"/>
                 <c:pt idx="0">
                   <c:v>40848</c:v>
                 </c:pt>
@@ -641,16 +641,91 @@
                 </c:pt>
                 <c:pt idx="144">
                   <c:v>45231</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>45261</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>45292</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>45323</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>45352</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>45383</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>45413</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>45444</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>45474</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>45505</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>45536</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>45566</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>45597</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>45627</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>45717</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>45748</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>45778</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>45809</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>45839</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>45870</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>45901</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>45931</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>45962</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>45992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$149</c:f>
+              <c:f>Sheet1!$B$5:$B$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="145"/>
+                <c:ptCount val="170"/>
                 <c:pt idx="0">
                   <c:v>329</c:v>
                 </c:pt>
@@ -689,6 +764,12 @@
                 </c:pt>
                 <c:pt idx="143">
                   <c:v>13717</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>15683</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>18300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -874,7 +955,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -961,10 +1042,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$149</c:f>
+              <c:f>Sheet1!$A$5:$A$174</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="145"/>
+                <c:ptCount val="170"/>
                 <c:pt idx="0">
                   <c:v>40848</c:v>
                 </c:pt>
@@ -1399,16 +1480,91 @@
                 </c:pt>
                 <c:pt idx="144">
                   <c:v>45231</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>45261</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>45292</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>45323</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>45352</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>45383</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>45413</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>45444</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>45474</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>45505</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>45536</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>45566</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>45597</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>45627</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>45717</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>45748</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>45778</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>45809</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>45839</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>45870</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>45901</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>45931</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>45962</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>45992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$149</c:f>
+              <c:f>Sheet1!$C$5:$C$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="145"/>
+                <c:ptCount val="170"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
@@ -1447,6 +1603,12 @@
                 </c:pt>
                 <c:pt idx="143">
                   <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1632,7 +1794,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3960,9 +4122,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4000,7 +4162,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4106,7 +4268,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4248,7 +4410,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4256,10 +4418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CD39B4-C474-484D-A525-0FA885BAEB22}">
-  <dimension ref="A4:D158"/>
+  <dimension ref="A4:D183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126:B148"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5196,6 +5358,143 @@
         <v>45505</v>
       </c>
     </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>45566</v>
+      </c>
+      <c r="B160">
+        <v>15683</v>
+      </c>
+      <c r="C160">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>45597</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>45627</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" s="1">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" s="1">
+        <v>45689</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" s="1">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" s="1">
+        <v>45778</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" s="1">
+        <v>45809</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" s="1">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" s="1">
+        <v>45870</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>45901</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" s="1">
+        <v>45931</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" s="1">
+        <v>45962</v>
+      </c>
+      <c r="B173">
+        <v>18300</v>
+      </c>
+      <c r="C173">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" s="1">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" s="1">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" s="1">
+        <v>46082</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" s="1">
+        <v>46113</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" s="1">
+        <v>46143</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" s="1">
+        <v>46174</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" s="1">
+        <v>46204</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>46235</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
+        <v>46266</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>